<commit_message>
New updates of FMD simulation
</commit_message>
<xml_diff>
--- a/Data/Latest-03-24/CalfCrop.xlsx
+++ b/Data/Latest-03-24/CalfCrop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dinesh/Dinesh/Research/CattleModel/Data/Latest-03-24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C83ADE9E-3732-AB47-AE64-94B5F1CC2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{125BB327-B1C3-A844-BBBB-0E9FA9C288EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="6760" yWindow="7520" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CalfCrop" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -952,12 +952,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="17" max="17" width="36.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>